<commit_message>
feature: connect database and design api
</commit_message>
<xml_diff>
--- a/docs/planning/planning.xlsx
+++ b/docs/planning/planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\phuongtran\code\training\PanasonicRDTraining-backend-java\docs\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3AF96F-5CA8-494A-BE6E-5727EE11DBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CF47D9-AAEB-44B0-82AB-2B5A85CC36E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CCF18E85-42DE-43CA-AF03-66615B9E3C26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>JAVA TRAINING PLANNING</t>
   </si>
@@ -84,13 +84,6 @@
     <t>Environment setup</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Design API
- - Implement API</t>
-  </si>
-  <si>
-    <t>Design and implement endpoints</t>
-  </si>
-  <si>
     <t>2 day</t>
   </si>
   <si>
@@ -137,6 +130,46 @@
   </si>
   <si>
     <t xml:space="preserve">All previous </t>
+  </si>
+  <si>
+    <t>Java research</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Review Java
+ - Learn about Spring Boot</t>
+  </si>
+  <si>
+    <t>Learn Java and Spring framework</t>
+  </si>
+  <si>
+    <t>API design</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Design API </t>
+  </si>
+  <si>
+    <t>Design API, get and fix according to feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Connect database
+ - Implement API
+ - Write unit test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement endpoints with data from database and test </t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>28/10/2025</t>
+  </si>
+  <si>
+    <t>29/10/2025</t>
+  </si>
+  <si>
+    <t>Database setup
+API design</t>
   </si>
 </sst>
 </file>
@@ -238,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -250,10 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -263,6 +296,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464176AE-8AD7-4108-A410-638A158C1B30}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,11 +644,11 @@
     <col min="1" max="1" width="25.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="21.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -620,8 +656,9 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-    </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="6"/>
+    </row>
+    <row r="3" spans="1:9" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -635,10 +672,13 @@
         <v>4</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -651,9 +691,12 @@
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -667,107 +710,162 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="10">
+        <v>45727</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="10">
+        <v>45758</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="10">
+        <v>45757</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="10">
+        <v>45818</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="10">
+        <v>45849</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="10">
+        <v>45911</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="E12" s="10">
+        <v>45941</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>